<commit_message>
Add group to header file PCHS app
</commit_message>
<xml_diff>
--- a/quarterlyReports/mammograms/header_file_mammogram.xlsx
+++ b/quarterlyReports/mammograms/header_file_mammogram.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mayalapp/Documents/coding_projects/dad_data_project/quarterlyReports/mammograms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FC96F4-4EA2-5B4D-B6F8-DA96AAEBF57E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14487626-88EC-7C41-A1A5-C318847766C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="13960" xr2:uid="{A3C09648-A85F-004C-88D6-616841BE841B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Screened patients: Patients that received a mammogram during the 2 years prior to the end of the reporting period.</t>
   </si>
@@ -49,13 +49,19 @@
   </si>
   <si>
     <t>Report type</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Site</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -71,15 +77,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <name val="Microsoft Sans Serif"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <name val="Microsoft Sans Serif"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,11 +118,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E731B5D-8C6F-4B45-B462-14B88FDFFF33}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,9 +466,17 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>